<commit_message>
bubble plot, plot download, and hyperlinks
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data11.xlsx
+++ b/GW_seaweed_seasonality_transect_data11.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25506"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25518"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="668" documentId="8_{BF71311B-6A6D-4ED2-9B6E-E3E672618DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B3480CC-A344-439E-AE98-24AD564C7838}"/>
+  <xr:revisionPtr revIDLastSave="692" documentId="8_{BF71311B-6A6D-4ED2-9B6E-E3E672618DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12936EE6-8C0D-450E-800D-08135894613A}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,11 +1134,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB435"/>
+  <dimension ref="A1:BB478"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AZ353" sqref="AZ353"/>
+      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A433" sqref="A433:A478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="14.45"/>
@@ -16984,10 +16984,769 @@
       </c>
     </row>
     <row r="434" spans="1:50" ht="15">
-      <c r="A434" s="1"/>
+      <c r="A434" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B434">
+        <v>7</v>
+      </c>
+      <c r="C434">
+        <v>14</v>
+      </c>
+      <c r="D434">
+        <v>2</v>
+      </c>
+      <c r="E434" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="435" spans="1:50" ht="15">
-      <c r="A435" s="1"/>
+      <c r="A435" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B435">
+        <v>7</v>
+      </c>
+      <c r="C435">
+        <v>14</v>
+      </c>
+      <c r="D435">
+        <v>2</v>
+      </c>
+      <c r="E435" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="436" spans="1:50" ht="15">
+      <c r="A436" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B436">
+        <v>7</v>
+      </c>
+      <c r="C436">
+        <v>14</v>
+      </c>
+      <c r="D436">
+        <v>2</v>
+      </c>
+      <c r="E436" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="437" spans="1:50" ht="15">
+      <c r="A437" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B437">
+        <v>7</v>
+      </c>
+      <c r="C437">
+        <v>14</v>
+      </c>
+      <c r="D437">
+        <v>2</v>
+      </c>
+      <c r="E437" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="438" spans="1:50" ht="15">
+      <c r="A438" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B438">
+        <v>7</v>
+      </c>
+      <c r="C438">
+        <v>14</v>
+      </c>
+      <c r="D438">
+        <v>2</v>
+      </c>
+      <c r="E438" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="439" spans="1:50" ht="15">
+      <c r="A439" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B439">
+        <v>7</v>
+      </c>
+      <c r="C439">
+        <v>14</v>
+      </c>
+      <c r="D439">
+        <v>2</v>
+      </c>
+      <c r="E439" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="440" spans="1:50" ht="15">
+      <c r="A440" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B440">
+        <v>7</v>
+      </c>
+      <c r="C440">
+        <v>14</v>
+      </c>
+      <c r="D440">
+        <v>2</v>
+      </c>
+      <c r="E440" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="441" spans="1:50" ht="15">
+      <c r="A441" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B441">
+        <v>7</v>
+      </c>
+      <c r="C441">
+        <v>14</v>
+      </c>
+      <c r="D441">
+        <v>2</v>
+      </c>
+      <c r="E441" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="442" spans="1:50" ht="15">
+      <c r="A442" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B442">
+        <v>7</v>
+      </c>
+      <c r="C442">
+        <v>14</v>
+      </c>
+      <c r="D442">
+        <v>2</v>
+      </c>
+      <c r="E442" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="443" spans="1:50" ht="15">
+      <c r="A443" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B443">
+        <v>7</v>
+      </c>
+      <c r="C443">
+        <v>14</v>
+      </c>
+      <c r="D443">
+        <v>3</v>
+      </c>
+      <c r="E443" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:50" ht="15">
+      <c r="A444" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B444">
+        <v>7</v>
+      </c>
+      <c r="C444">
+        <v>14</v>
+      </c>
+      <c r="D444">
+        <v>3</v>
+      </c>
+      <c r="E444" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="445" spans="1:50" ht="15">
+      <c r="A445" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B445">
+        <v>7</v>
+      </c>
+      <c r="C445">
+        <v>14</v>
+      </c>
+      <c r="D445">
+        <v>3</v>
+      </c>
+      <c r="E445" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="446" spans="1:50" ht="15">
+      <c r="A446" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B446">
+        <v>7</v>
+      </c>
+      <c r="C446">
+        <v>14</v>
+      </c>
+      <c r="D446">
+        <v>3</v>
+      </c>
+      <c r="E446" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="447" spans="1:50" ht="15">
+      <c r="A447" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B447">
+        <v>7</v>
+      </c>
+      <c r="C447">
+        <v>14</v>
+      </c>
+      <c r="D447">
+        <v>3</v>
+      </c>
+      <c r="E447" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="448" spans="1:50" ht="15">
+      <c r="A448" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B448">
+        <v>7</v>
+      </c>
+      <c r="C448">
+        <v>14</v>
+      </c>
+      <c r="D448">
+        <v>3</v>
+      </c>
+      <c r="E448" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" ht="15">
+      <c r="A449" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B449">
+        <v>7</v>
+      </c>
+      <c r="C449">
+        <v>14</v>
+      </c>
+      <c r="D449">
+        <v>3</v>
+      </c>
+      <c r="E449" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" ht="15">
+      <c r="A450" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B450">
+        <v>7</v>
+      </c>
+      <c r="C450">
+        <v>14</v>
+      </c>
+      <c r="D450">
+        <v>3</v>
+      </c>
+      <c r="E450" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" ht="15">
+      <c r="A451" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B451">
+        <v>7</v>
+      </c>
+      <c r="C451">
+        <v>14</v>
+      </c>
+      <c r="D451">
+        <v>3</v>
+      </c>
+      <c r="E451" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" ht="15">
+      <c r="A452" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B452">
+        <v>7</v>
+      </c>
+      <c r="C452">
+        <v>14</v>
+      </c>
+      <c r="D452">
+        <v>3</v>
+      </c>
+      <c r="E452" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" ht="15">
+      <c r="A453" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B453">
+        <v>7</v>
+      </c>
+      <c r="C453">
+        <v>14</v>
+      </c>
+      <c r="D453">
+        <v>3</v>
+      </c>
+      <c r="E453" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" ht="15">
+      <c r="A454" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B454">
+        <v>7</v>
+      </c>
+      <c r="C454">
+        <v>14</v>
+      </c>
+      <c r="D454">
+        <v>3</v>
+      </c>
+      <c r="E454" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" ht="15">
+      <c r="A455" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B455">
+        <v>7</v>
+      </c>
+      <c r="C455">
+        <v>14</v>
+      </c>
+      <c r="D455">
+        <v>3</v>
+      </c>
+      <c r="E455" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" ht="15">
+      <c r="A456" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B456">
+        <v>7</v>
+      </c>
+      <c r="C456">
+        <v>14</v>
+      </c>
+      <c r="D456">
+        <v>3</v>
+      </c>
+      <c r="E456" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" ht="15">
+      <c r="A457" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B457">
+        <v>7</v>
+      </c>
+      <c r="C457">
+        <v>14</v>
+      </c>
+      <c r="D457">
+        <v>3</v>
+      </c>
+      <c r="E457" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" ht="15">
+      <c r="A458" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B458">
+        <v>7</v>
+      </c>
+      <c r="C458">
+        <v>14</v>
+      </c>
+      <c r="D458">
+        <v>3</v>
+      </c>
+      <c r="E458" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" ht="15">
+      <c r="A459" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B459">
+        <v>7</v>
+      </c>
+      <c r="C459">
+        <v>14</v>
+      </c>
+      <c r="D459">
+        <v>3</v>
+      </c>
+      <c r="E459" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" ht="15">
+      <c r="A460" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B460">
+        <v>7</v>
+      </c>
+      <c r="C460">
+        <v>14</v>
+      </c>
+      <c r="D460">
+        <v>3</v>
+      </c>
+      <c r="E460">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" ht="15">
+      <c r="A461" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B461">
+        <v>7</v>
+      </c>
+      <c r="C461">
+        <v>14</v>
+      </c>
+      <c r="D461">
+        <v>3</v>
+      </c>
+      <c r="E461">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" ht="15">
+      <c r="A462" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B462">
+        <v>7</v>
+      </c>
+      <c r="C462">
+        <v>14</v>
+      </c>
+      <c r="D462">
+        <v>4</v>
+      </c>
+      <c r="E462" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" ht="15">
+      <c r="A463" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B463">
+        <v>7</v>
+      </c>
+      <c r="C463">
+        <v>14</v>
+      </c>
+      <c r="D463">
+        <v>4</v>
+      </c>
+      <c r="E463" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" ht="15">
+      <c r="A464" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B464">
+        <v>7</v>
+      </c>
+      <c r="C464">
+        <v>14</v>
+      </c>
+      <c r="D464">
+        <v>4</v>
+      </c>
+      <c r="E464" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" ht="15">
+      <c r="A465" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B465">
+        <v>7</v>
+      </c>
+      <c r="C465">
+        <v>14</v>
+      </c>
+      <c r="D465">
+        <v>4</v>
+      </c>
+      <c r="E465" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" ht="15">
+      <c r="A466" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B466">
+        <v>7</v>
+      </c>
+      <c r="C466">
+        <v>14</v>
+      </c>
+      <c r="D466">
+        <v>4</v>
+      </c>
+      <c r="E466" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" ht="15">
+      <c r="A467" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B467">
+        <v>7</v>
+      </c>
+      <c r="C467">
+        <v>14</v>
+      </c>
+      <c r="D467">
+        <v>4</v>
+      </c>
+      <c r="E467" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" ht="15">
+      <c r="A468" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B468">
+        <v>7</v>
+      </c>
+      <c r="C468">
+        <v>14</v>
+      </c>
+      <c r="D468">
+        <v>4</v>
+      </c>
+      <c r="E468" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" ht="15">
+      <c r="A469" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B469">
+        <v>7</v>
+      </c>
+      <c r="C469">
+        <v>14</v>
+      </c>
+      <c r="D469">
+        <v>4</v>
+      </c>
+      <c r="E469" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" ht="15">
+      <c r="A470" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B470">
+        <v>7</v>
+      </c>
+      <c r="C470">
+        <v>14</v>
+      </c>
+      <c r="D470">
+        <v>4</v>
+      </c>
+      <c r="E470" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" ht="15">
+      <c r="A471" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B471">
+        <v>7</v>
+      </c>
+      <c r="C471">
+        <v>14</v>
+      </c>
+      <c r="D471">
+        <v>4</v>
+      </c>
+      <c r="E471" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" ht="15">
+      <c r="A472" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B472">
+        <v>7</v>
+      </c>
+      <c r="C472">
+        <v>14</v>
+      </c>
+      <c r="D472">
+        <v>4</v>
+      </c>
+      <c r="E472" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" ht="15">
+      <c r="A473" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B473">
+        <v>7</v>
+      </c>
+      <c r="C473">
+        <v>14</v>
+      </c>
+      <c r="D473">
+        <v>4</v>
+      </c>
+      <c r="E473" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" ht="15">
+      <c r="A474" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B474">
+        <v>7</v>
+      </c>
+      <c r="C474">
+        <v>14</v>
+      </c>
+      <c r="D474">
+        <v>4</v>
+      </c>
+      <c r="E474" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" ht="15">
+      <c r="A475" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B475">
+        <v>7</v>
+      </c>
+      <c r="C475">
+        <v>14</v>
+      </c>
+      <c r="D475">
+        <v>4</v>
+      </c>
+      <c r="E475" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" ht="15">
+      <c r="A476" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B476">
+        <v>7</v>
+      </c>
+      <c r="C476">
+        <v>14</v>
+      </c>
+      <c r="D476">
+        <v>4</v>
+      </c>
+      <c r="E476" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" ht="15">
+      <c r="A477" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B477">
+        <v>7</v>
+      </c>
+      <c r="C477">
+        <v>14</v>
+      </c>
+      <c r="D477">
+        <v>4</v>
+      </c>
+      <c r="E477" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" ht="15">
+      <c r="A478" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B478">
+        <v>7</v>
+      </c>
+      <c r="C478">
+        <v>14</v>
+      </c>
+      <c r="D478">
+        <v>4</v>
+      </c>
+      <c r="E478" s="1">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>